<commit_message>
Penambahan Automation Testing API
</commit_message>
<xml_diff>
--- a/DataPaketId.xlsx
+++ b/DataPaketId.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Katalon Studio\PT Paket Informasi Digital(paket.id)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56DA2A8-373E-4CBC-AA45-52F779CB9735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24286B62-A302-4409-9567-8E99DC30644E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{96E3ECDB-4F70-4973-98A7-42A33FA1FED1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
   <si>
     <t>Nama</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>The full name field is require</t>
   </si>
   <si>
     <t>Scenario</t>
@@ -666,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A7B81E-2245-4131-BC18-1A3FD0CCCDF7}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +681,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -708,164 +705,164 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>85772272212</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
         <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>872272215</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="D4" s="1">
         <v>123</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="1">
         <v>85772272212</v>
       </c>
       <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1">
         <v>85772272281</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>1234567</v>
@@ -880,300 +877,300 @@
         <v>1234567890</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" t="s">
         <v>56</v>
       </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
-        <v>67</v>
-      </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
         <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
       </c>
       <c r="C16" s="1">
         <v>52612712</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="E16" t="s">
-        <v>71</v>
-      </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" t="s">
         <v>75</v>
       </c>
-      <c r="E17" t="s">
-        <v>76</v>
-      </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" t="s">
         <v>80</v>
       </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>12340974</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" t="s">
         <v>12</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
         <v>13</v>
       </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>